<commit_message>
Modif doc prod + Prefab Grid et background
</commit_message>
<xml_diff>
--- a/DocumentProd/E-art Sudoku Production Document.xlsx
+++ b/DocumentProd/E-art Sudoku Production Document.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\E-artSudoku\E-art-Sudoku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\E-art-Sudoku\DocumentProd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,33 +59,6 @@
     <t>10min</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Création d'une brique : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Carré avec quadrillage 3*3
-6 chiffres placé dans 6 cases
-3 cases blanches
-Création du prefab Unity</t>
-    </r>
-  </si>
-  <si>
     <t>Tristan</t>
   </si>
   <si>
@@ -186,31 +159,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Coder le bouton valider :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Check si le joueur rempli les conditions de victoire (cf Game Concept)
-Si oui =&gt; écran de victoire                 Si non =&gt; Apparition de "l'écran faute"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Coder écran de victoire :</t>
     </r>
     <r>
@@ -315,6 +263,59 @@
       </rPr>
       <t xml:space="preserve">
 Savoir si le joueur a bien mit le résultat attendu dans la case</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Création d'une brique : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Carré avec quadrillage 3*3
+Chiffres placé dans les cases
+Cases blanches
+Création du prefab Unity</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Coder le bouton valider et éffacer :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Check si le joueur rempli les conditions de victoire (cf Game Concept)
+Si oui =&gt; écran de victoire                 Si non =&gt; Apparition de "l'écran faute"
+Remettre à zero le niveau</t>
     </r>
   </si>
 </sst>
@@ -722,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95FFB01-6617-4B66-BBD3-6D61DB0958A4}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,10 +742,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -778,17 +779,17 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="6"/>
       <c r="G7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -799,7 +800,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -809,10 +810,10 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -823,20 +824,20 @@
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6"/>
       <c r="G9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -844,23 +845,23 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="6"/>
       <c r="G10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
         <v>23</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -868,23 +869,23 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" s="7"/>
       <c r="G11" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -892,36 +893,36 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="6"/>
       <c r="G13" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -929,13 +930,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E14" s="6"/>
       <c r="G14" s="3" t="s">

</xml_diff>

<commit_message>
Doc de prod modif
</commit_message>
<xml_diff>
--- a/DocumentProd/E-art Sudoku Production Document.xlsx
+++ b/DocumentProd/E-art Sudoku Production Document.xlsx
@@ -332,13 +332,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +346,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -363,12 +363,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -383,7 +383,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
@@ -403,13 +403,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Satisfaisant" xfId="2" builtinId="26"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -784,7 +784,7 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="6"/>
       <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
@@ -853,7 +853,7 @@
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="7"/>
       <c r="G10" s="3" t="s">
         <v>21</v>
       </c>
@@ -877,7 +877,7 @@
       <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
       <c r="G11" s="3" t="s">
         <v>23</v>
       </c>
@@ -901,7 +901,7 @@
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Document de production phase 2
</commit_message>
<xml_diff>
--- a/DocumentProd/E-art Sudoku Production Document.xlsx
+++ b/DocumentProd/E-art Sudoku Production Document.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\E-art-Sudoku\DocumentProd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\E-artSudoku\E-art-Sudoku\DocumentProd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>E-art Sudoku document de production</t>
   </si>
@@ -318,12 +318,209 @@
 Remettre à zero le niveau</t>
     </r>
   </si>
+  <si>
+    <t>PHASE 1</t>
+  </si>
+  <si>
+    <t>PHASE 2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Amélioration d'UI :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sprite bouton quitter
+Sprite bouton jouer
+Sprite bouton valider
+Sprite bouton effacer
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Graph + code</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ajout d'une musique de fond :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Choisir une musique
+Intégrer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ajout d'un d'icone de lancement :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Création de l'icone
+Intégration</t>
+    </r>
+  </si>
+  <si>
+    <t>Audio + code</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ajout d'un bouton quitter In-Game :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Sprite bouton
+Code bouton (Ramène au menu)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>(Bonus)</t>
+  </si>
+  <si>
+    <t>20min</t>
+  </si>
+  <si>
+    <t>Seb + Kevin</t>
+  </si>
+  <si>
+    <t>5min</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ajout d'un nouveau niveau :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Choix du sudoku
+Intégration
+Bouton "continuer" en fin de niveau
+Détecter à quel niveau est le joueur (ne pas afficher "continuer" s'il est au dernier niveau)
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Feedback sonore :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Choix d'un bruitage
+Code déclanchement du son (quand le bouton est pressé)</t>
+    </r>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>1h20min</t>
+  </si>
+  <si>
+    <t>1h05min</t>
+  </si>
+  <si>
+    <t>TACHES A COMMENCER SEULEMENT 
+SI TOUT EST OK</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +543,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +569,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -369,11 +586,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,8 +609,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -706,14 +933,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95FFB01-6617-4B66-BBD3-6D61DB0958A4}">
-  <dimension ref="A2:K21"/>
+  <dimension ref="A2:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="65.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
@@ -733,6 +961,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
@@ -935,22 +1168,190 @@
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="G20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="G21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="G22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="G23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="G24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>